<commit_message>
nutrients and details added
</commit_message>
<xml_diff>
--- a/assets/Sir Mubarak data/Categorized Feeds 2-1 (1) Cleaned.xlsx
+++ b/assets/Sir Mubarak data/Categorized Feeds 2-1 (1) Cleaned.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Composition Sheet" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="clean composition" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="64">
   <si>
     <t>Category 1</t>
   </si>
@@ -206,9 +207,6 @@
     <t>Price per kg</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -225,6 +223,9 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>ME raw</t>
   </si>
 </sst>
 </file>
@@ -329,7 +330,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -364,7 +365,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -549,38 +550,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I40"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection sqref="A1:H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="4" max="5" width="6" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>60</v>
@@ -591,1138 +590,1057 @@
       <c r="H1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="B2">
+        <v>12.5</v>
       </c>
       <c r="C2">
-        <v>12.5</v>
+        <v>23.5</v>
       </c>
       <c r="D2">
-        <v>63.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E2">
-        <v>23.5</v>
+        <f>D2*1000</f>
+        <v>2300</v>
       </c>
       <c r="F2">
-        <v>2.2999999999999998</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H2">
-        <v>10</v>
-      </c>
-      <c r="I2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
+      <c r="B3">
+        <v>23.3</v>
       </c>
       <c r="C3">
-        <v>23.3</v>
+        <v>8.9</v>
       </c>
       <c r="D3">
-        <v>61.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E3">
-        <v>8.9</v>
+        <f t="shared" ref="E3:E40" si="0">D3*1000</f>
+        <v>2200</v>
       </c>
       <c r="F3">
-        <v>2.2000000000000002</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="I3">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>1</v>
+      <c r="B4">
+        <v>26.3</v>
       </c>
       <c r="C4">
-        <v>26.3</v>
+        <v>14.2</v>
       </c>
       <c r="D4">
-        <v>66.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E4">
-        <v>14.2</v>
+        <f t="shared" si="0"/>
+        <v>2300</v>
       </c>
       <c r="F4">
-        <v>2.2999999999999998</v>
+        <v>5</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
-        <v>1</v>
+      <c r="B5">
+        <v>11.5</v>
       </c>
       <c r="C5">
-        <v>11.5</v>
+        <v>23</v>
       </c>
       <c r="D5">
-        <v>56.8</v>
+        <v>2.1</v>
       </c>
       <c r="E5">
-        <v>23</v>
+        <f t="shared" si="0"/>
+        <v>2100</v>
       </c>
       <c r="F5">
-        <v>2.1</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H5">
-        <v>10</v>
-      </c>
-      <c r="I5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>1</v>
+      <c r="B6">
+        <v>29.6</v>
       </c>
       <c r="C6">
-        <v>29.6</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D6">
-        <v>62.6</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E6">
-        <v>9.6999999999999993</v>
+        <f t="shared" si="0"/>
+        <v>2300</v>
       </c>
       <c r="F6">
-        <v>2.2999999999999998</v>
+        <v>10</v>
       </c>
       <c r="G6">
         <v>10</v>
       </c>
       <c r="H6">
-        <v>10</v>
-      </c>
-      <c r="I6">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
-        <v>1</v>
+      <c r="B7">
+        <v>23.2</v>
       </c>
       <c r="C7">
-        <v>23.2</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>60.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>2200</v>
       </c>
       <c r="F7">
-        <v>2.2000000000000002</v>
+        <v>5</v>
       </c>
       <c r="G7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H7">
-        <v>10</v>
-      </c>
-      <c r="I7">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
-        <v>1</v>
+      <c r="B8">
+        <v>26.8</v>
       </c>
       <c r="C8">
-        <v>26.8</v>
+        <v>6.4</v>
       </c>
       <c r="D8">
-        <v>45.8</v>
+        <v>1.7</v>
       </c>
       <c r="E8">
-        <v>6.4</v>
+        <f t="shared" si="0"/>
+        <v>1700</v>
       </c>
       <c r="F8">
-        <v>1.7</v>
+        <v>3</v>
       </c>
       <c r="G8">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H8">
-        <v>10</v>
-      </c>
-      <c r="I8">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s">
-        <v>1</v>
+      <c r="B9">
+        <v>17.899999999999999</v>
       </c>
       <c r="C9">
-        <v>17.899999999999999</v>
+        <v>11.6</v>
       </c>
       <c r="D9">
-        <v>62.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E9">
-        <v>11.6</v>
+        <f t="shared" si="0"/>
+        <v>2300</v>
       </c>
       <c r="F9">
-        <v>2.2999999999999998</v>
+        <v>5</v>
       </c>
       <c r="G9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H9">
-        <v>10</v>
-      </c>
-      <c r="I9">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
-        <v>32</v>
+      <c r="B10">
+        <v>91</v>
       </c>
       <c r="C10">
-        <v>91</v>
+        <v>4.8</v>
       </c>
       <c r="D10">
-        <v>41.5</v>
+        <v>1.5</v>
       </c>
       <c r="E10">
-        <v>4.8</v>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="F10">
-        <v>1.5</v>
+        <v>17</v>
       </c>
       <c r="G10">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H10">
-        <v>10</v>
-      </c>
-      <c r="I10">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
-        <v>32</v>
+      <c r="B11">
+        <v>92.8</v>
       </c>
       <c r="C11">
-        <v>92.8</v>
+        <v>5.5</v>
       </c>
       <c r="D11">
-        <v>47.9</v>
+        <v>1.7</v>
       </c>
       <c r="E11">
-        <v>5.5</v>
+        <f t="shared" si="0"/>
+        <v>1700</v>
       </c>
       <c r="F11">
-        <v>1.7</v>
+        <v>8</v>
       </c>
       <c r="G11">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H11">
-        <v>10</v>
-      </c>
-      <c r="I11">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
-        <v>32</v>
+      <c r="B12">
+        <v>93.1</v>
       </c>
       <c r="C12">
-        <v>93.1</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>41.8</v>
+        <v>1.5</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="F12">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="G12">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H12">
-        <v>10</v>
-      </c>
-      <c r="I12">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" t="s">
-        <v>32</v>
+      <c r="B13">
+        <v>92.9</v>
       </c>
       <c r="C13">
-        <v>92.9</v>
+        <v>6.2</v>
       </c>
       <c r="D13">
-        <v>42.5</v>
+        <v>1.5</v>
       </c>
       <c r="E13">
-        <v>6.2</v>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="F13">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="G13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H13">
-        <v>10</v>
-      </c>
-      <c r="I13">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" t="s">
-        <v>32</v>
+      <c r="B14">
+        <v>85.5</v>
       </c>
       <c r="C14">
-        <v>85.5</v>
+        <v>6.6</v>
       </c>
       <c r="D14">
-        <v>48.5</v>
+        <v>1.8</v>
       </c>
       <c r="E14">
-        <v>6.6</v>
+        <f t="shared" si="0"/>
+        <v>1800</v>
       </c>
       <c r="F14">
-        <v>1.8</v>
+        <v>5</v>
       </c>
       <c r="G14">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H14">
-        <v>10</v>
-      </c>
-      <c r="I14">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="B15" t="s">
-        <v>32</v>
+      <c r="B15">
+        <v>91.5</v>
       </c>
       <c r="C15">
-        <v>91.5</v>
+        <v>3.7</v>
       </c>
       <c r="D15">
-        <v>58.7</v>
+        <v>1.9</v>
       </c>
       <c r="E15">
-        <v>3.7</v>
+        <f t="shared" si="0"/>
+        <v>1900</v>
       </c>
       <c r="F15">
-        <v>1.9</v>
+        <v>5</v>
       </c>
       <c r="G15">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H15">
-        <v>10</v>
-      </c>
-      <c r="I15">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
-      <c r="B16" t="s">
-        <v>32</v>
+      <c r="B16">
+        <v>91.9</v>
       </c>
       <c r="C16">
-        <v>91.9</v>
+        <v>3.9</v>
       </c>
       <c r="D16">
-        <v>42.5</v>
+        <v>1.5</v>
       </c>
       <c r="E16">
-        <v>3.9</v>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="F16">
-        <v>1.5</v>
+        <v>15</v>
       </c>
       <c r="G16">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H16">
-        <v>10</v>
-      </c>
-      <c r="I16">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
-      <c r="B17" t="s">
-        <v>11</v>
+      <c r="B17">
+        <v>87.3</v>
       </c>
       <c r="C17">
-        <v>87.3</v>
+        <v>9.1</v>
       </c>
       <c r="D17">
-        <v>88.1</v>
+        <v>3.2</v>
       </c>
       <c r="E17">
-        <v>9.1</v>
+        <f t="shared" si="0"/>
+        <v>3200</v>
       </c>
       <c r="F17">
-        <v>3.2</v>
+        <v>75</v>
       </c>
       <c r="G17">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="H17">
-        <v>10</v>
-      </c>
-      <c r="I17">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B18" t="s">
-        <v>11</v>
+      <c r="B18">
+        <v>87</v>
       </c>
       <c r="C18">
-        <v>87</v>
+        <v>14.4</v>
       </c>
       <c r="D18">
-        <v>88.3</v>
+        <v>3.2</v>
       </c>
       <c r="E18">
-        <v>14.4</v>
+        <f t="shared" si="0"/>
+        <v>3200</v>
       </c>
       <c r="F18">
-        <v>3.2</v>
+        <v>100</v>
       </c>
       <c r="G18">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="H18">
-        <v>10</v>
-      </c>
-      <c r="I18">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
-        <v>11</v>
+      <c r="B19">
+        <v>89.6</v>
       </c>
       <c r="C19">
-        <v>89.6</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="D19">
-        <v>86.7</v>
+        <v>3.1</v>
       </c>
       <c r="E19">
-        <v>9.3000000000000007</v>
+        <f t="shared" si="0"/>
+        <v>3100</v>
       </c>
       <c r="F19">
-        <v>3.1</v>
+        <v>100</v>
       </c>
       <c r="G19">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="H19">
-        <v>10</v>
-      </c>
-      <c r="I19">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>41</v>
       </c>
-      <c r="B20" t="s">
-        <v>11</v>
+      <c r="B20">
+        <v>87.5</v>
       </c>
       <c r="C20">
-        <v>87.5</v>
+        <v>12.8</v>
       </c>
       <c r="D20">
-        <v>79.8</v>
+        <v>2.9</v>
       </c>
       <c r="E20">
-        <v>12.8</v>
+        <f t="shared" si="0"/>
+        <v>2900</v>
       </c>
       <c r="F20">
-        <v>2.9</v>
+        <v>50</v>
       </c>
       <c r="G20">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="H20">
-        <v>10</v>
-      </c>
-      <c r="I20">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
-      <c r="B21" t="s">
-        <v>11</v>
+      <c r="B21">
+        <v>89</v>
       </c>
       <c r="C21">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="D21">
-        <v>73.099999999999994</v>
+        <v>2.6</v>
       </c>
       <c r="E21">
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>2600</v>
       </c>
       <c r="F21">
-        <v>2.6</v>
+        <v>50</v>
       </c>
       <c r="G21">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="H21">
-        <v>10</v>
-      </c>
-      <c r="I21">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
-        <v>11</v>
+      <c r="B22">
+        <v>87</v>
       </c>
       <c r="C22">
-        <v>87</v>
+        <v>15.9</v>
       </c>
       <c r="D22">
-        <v>78.099999999999994</v>
+        <v>2.8</v>
       </c>
       <c r="E22">
-        <v>15.9</v>
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="F22">
-        <v>2.8</v>
+        <v>45</v>
       </c>
       <c r="G22">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="H22">
-        <v>10</v>
-      </c>
-      <c r="I22">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
-      <c r="B23" t="s">
-        <v>11</v>
+      <c r="B23">
+        <v>90.2</v>
       </c>
       <c r="C23">
-        <v>90.2</v>
+        <v>15.9</v>
       </c>
       <c r="D23">
-        <v>76.400000000000006</v>
+        <v>2.8</v>
       </c>
       <c r="E23">
-        <v>15.9</v>
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="F23">
-        <v>2.8</v>
+        <v>30</v>
       </c>
       <c r="G23">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H23">
-        <v>10</v>
-      </c>
-      <c r="I23">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
-      <c r="B24" t="s">
-        <v>11</v>
+      <c r="B24">
+        <v>21</v>
       </c>
       <c r="C24">
-        <v>21</v>
+        <v>10.7</v>
       </c>
       <c r="D24">
-        <v>66.099999999999994</v>
+        <v>2.4</v>
       </c>
       <c r="E24">
-        <v>10.7</v>
+        <f t="shared" si="0"/>
+        <v>2400</v>
       </c>
       <c r="F24">
-        <v>2.4</v>
+        <v>50</v>
       </c>
       <c r="G24">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="H24">
-        <v>10</v>
-      </c>
-      <c r="I24">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>40</v>
       </c>
-      <c r="B25" t="s">
-        <v>11</v>
+      <c r="B25">
+        <v>20.8</v>
       </c>
       <c r="C25">
-        <v>20.8</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D25">
-        <v>57.4</v>
+        <v>2.1</v>
       </c>
       <c r="E25">
-        <v>8.6999999999999993</v>
+        <f t="shared" si="0"/>
+        <v>2100</v>
       </c>
       <c r="F25">
-        <v>2.1</v>
+        <v>20</v>
       </c>
       <c r="G25">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H25">
-        <v>10</v>
-      </c>
-      <c r="I25">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
-      <c r="B26" t="s">
-        <v>11</v>
+      <c r="B26">
+        <v>23</v>
       </c>
       <c r="C26">
-        <v>23</v>
+        <v>10.3</v>
       </c>
       <c r="D26">
-        <v>70.3</v>
+        <v>2.5</v>
       </c>
       <c r="E26">
-        <v>10.3</v>
+        <f t="shared" si="0"/>
+        <v>2500</v>
       </c>
       <c r="F26">
-        <v>2.5</v>
+        <v>20</v>
       </c>
       <c r="G26">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H26">
-        <v>10</v>
-      </c>
-      <c r="I26">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
-      <c r="B27" t="s">
-        <v>11</v>
+      <c r="B27">
+        <v>89</v>
       </c>
       <c r="C27">
-        <v>89</v>
+        <v>15.3</v>
       </c>
       <c r="D27">
-        <v>65.099999999999994</v>
+        <v>2.4</v>
       </c>
       <c r="E27">
-        <v>15.3</v>
+        <f t="shared" si="0"/>
+        <v>2400</v>
       </c>
       <c r="F27">
-        <v>2.4</v>
+        <v>65</v>
       </c>
       <c r="G27">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="H27">
-        <v>10</v>
-      </c>
-      <c r="I27">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
-      <c r="B28" t="s">
-        <v>11</v>
+      <c r="B28">
+        <v>88.6</v>
       </c>
       <c r="C28">
-        <v>88.6</v>
+        <v>16.8</v>
       </c>
       <c r="D28">
-        <v>64.8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E28">
-        <v>16.8</v>
+        <f t="shared" si="0"/>
+        <v>2300</v>
       </c>
       <c r="F28">
-        <v>2.2999999999999998</v>
+        <v>65</v>
       </c>
       <c r="G28">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="H28">
-        <v>10</v>
-      </c>
-      <c r="I28">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
-      <c r="B29" t="s">
-        <v>11</v>
+      <c r="B29">
+        <v>87.9</v>
       </c>
       <c r="C29">
-        <v>87.9</v>
+        <v>17.5</v>
       </c>
       <c r="D29">
-        <v>70</v>
+        <v>2.5</v>
       </c>
       <c r="E29">
-        <v>17.5</v>
+        <f t="shared" si="0"/>
+        <v>2500</v>
       </c>
       <c r="F29">
-        <v>2.5</v>
+        <v>65</v>
       </c>
       <c r="G29">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="H29">
-        <v>10</v>
-      </c>
-      <c r="I29">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>49</v>
       </c>
-      <c r="B30" t="s">
-        <v>11</v>
+      <c r="B30">
+        <v>84</v>
       </c>
       <c r="C30">
-        <v>84</v>
+        <v>3.5</v>
       </c>
       <c r="D30">
-        <v>69.7</v>
+        <v>2.5</v>
       </c>
       <c r="E30">
-        <v>3.5</v>
+        <f t="shared" si="0"/>
+        <v>2500</v>
       </c>
       <c r="F30">
-        <v>2.5</v>
+        <v>20</v>
       </c>
       <c r="G30">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H30">
-        <v>10</v>
-      </c>
-      <c r="I30">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>38</v>
       </c>
-      <c r="B31" t="s">
-        <v>11</v>
+      <c r="B31">
+        <v>20.6</v>
       </c>
       <c r="C31">
-        <v>20.6</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="D31">
-        <v>12.3</v>
+        <v>2.8</v>
       </c>
       <c r="E31">
-        <v>78.599999999999994</v>
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="F31">
-        <v>2.8</v>
+        <v>20</v>
       </c>
       <c r="G31">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H31">
-        <v>10</v>
-      </c>
-      <c r="I31">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>17</v>
       </c>
-      <c r="B32" t="s">
-        <v>16</v>
+      <c r="B32">
+        <v>92.2</v>
       </c>
       <c r="C32">
-        <v>92.2</v>
+        <v>23.8</v>
       </c>
       <c r="D32">
-        <v>55.4</v>
+        <v>2</v>
       </c>
       <c r="E32">
-        <v>23.8</v>
+        <f t="shared" si="0"/>
+        <v>2000</v>
       </c>
       <c r="F32">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="G32">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="H32">
-        <v>10</v>
-      </c>
-      <c r="I32">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>18</v>
       </c>
-      <c r="B33" t="s">
-        <v>16</v>
+      <c r="B33">
+        <v>87.9</v>
       </c>
       <c r="C33">
-        <v>87.9</v>
+        <v>48</v>
       </c>
       <c r="D33">
-        <v>84.3</v>
+        <v>2.1</v>
       </c>
       <c r="E33">
-        <v>48</v>
+        <f t="shared" si="0"/>
+        <v>2100</v>
       </c>
       <c r="F33">
-        <v>2.1</v>
+        <v>300</v>
       </c>
       <c r="G33">
-        <v>300</v>
+        <v>10</v>
       </c>
       <c r="H33">
-        <v>10</v>
-      </c>
-      <c r="I33">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>19</v>
       </c>
-      <c r="B34" t="s">
-        <v>16</v>
+      <c r="B34">
+        <v>88.8</v>
       </c>
       <c r="C34">
-        <v>88.8</v>
+        <v>39.6</v>
       </c>
       <c r="D34">
-        <v>70.099999999999994</v>
+        <v>2.5</v>
       </c>
       <c r="E34">
-        <v>39.6</v>
+        <f t="shared" si="0"/>
+        <v>2500</v>
       </c>
       <c r="F34">
-        <v>2.5</v>
+        <v>145</v>
       </c>
       <c r="G34">
-        <v>145</v>
+        <v>10</v>
       </c>
       <c r="H34">
-        <v>10</v>
-      </c>
-      <c r="I34">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>20</v>
       </c>
-      <c r="B35" t="s">
-        <v>16</v>
+      <c r="B35">
+        <v>89.9</v>
       </c>
       <c r="C35">
-        <v>89.9</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="D35">
-        <v>73.5</v>
+        <v>2.7</v>
       </c>
       <c r="E35">
-        <v>34.299999999999997</v>
+        <f t="shared" si="0"/>
+        <v>2700</v>
       </c>
       <c r="F35">
-        <v>2.7</v>
+        <v>130</v>
       </c>
       <c r="G35">
-        <v>130</v>
+        <v>10</v>
       </c>
       <c r="H35">
-        <v>10</v>
-      </c>
-      <c r="I35">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>43</v>
       </c>
-      <c r="B36" t="s">
-        <v>16</v>
+      <c r="B36">
+        <v>88.3</v>
       </c>
       <c r="C36">
-        <v>88.3</v>
+        <v>29</v>
       </c>
       <c r="D36">
-        <v>77</v>
+        <v>2.8</v>
       </c>
       <c r="E36">
-        <v>29</v>
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="F36">
-        <v>2.8</v>
+        <v>61</v>
       </c>
       <c r="G36">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="H36">
-        <v>10</v>
-      </c>
-      <c r="I36">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
-      <c r="B37" t="s">
-        <v>16</v>
+      <c r="B37">
+        <v>90</v>
       </c>
       <c r="C37">
-        <v>90</v>
+        <v>59.7</v>
       </c>
       <c r="D37">
-        <v>78.099999999999994</v>
+        <v>2.8</v>
       </c>
       <c r="E37">
-        <v>59.7</v>
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="F37">
-        <v>2.8</v>
+        <v>40</v>
       </c>
       <c r="G37">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="H37">
-        <v>10</v>
-      </c>
-      <c r="I37">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>50</v>
       </c>
-      <c r="B38" t="s">
-        <v>16</v>
+      <c r="B38">
+        <v>91.2</v>
       </c>
       <c r="C38">
-        <v>91.2</v>
+        <v>17.8</v>
       </c>
       <c r="D38">
-        <v>61.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E38">
-        <v>17.8</v>
+        <f t="shared" si="0"/>
+        <v>2200</v>
       </c>
       <c r="F38">
-        <v>2.2000000000000002</v>
+        <v>50</v>
       </c>
       <c r="G38">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="H38">
-        <v>10</v>
-      </c>
-      <c r="I38">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>21</v>
       </c>
-      <c r="B39" t="s">
-        <v>16</v>
+      <c r="B39">
+        <v>89</v>
       </c>
       <c r="C39">
-        <v>89</v>
+        <v>32.5</v>
       </c>
       <c r="D39">
-        <v>58.4</v>
+        <v>2.1</v>
       </c>
       <c r="E39">
-        <v>32.5</v>
+        <f t="shared" si="0"/>
+        <v>2100</v>
       </c>
       <c r="F39">
-        <v>2.1</v>
+        <v>55</v>
       </c>
       <c r="G39">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="H39">
-        <v>10</v>
-      </c>
-      <c r="I39">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>23</v>
       </c>
-      <c r="B40" t="s">
-        <v>16</v>
+      <c r="B40">
+        <v>95</v>
       </c>
       <c r="C40">
-        <v>95</v>
+        <v>40.4</v>
       </c>
       <c r="D40">
-        <v>74</v>
+        <v>2.7</v>
       </c>
       <c r="E40">
-        <v>40.4</v>
+        <f t="shared" si="0"/>
+        <v>2700</v>
       </c>
       <c r="F40">
-        <v>2.7</v>
+        <v>120</v>
       </c>
       <c r="G40">
-        <v>120</v>
+        <v>10</v>
       </c>
       <c r="H40">
-        <v>10</v>
-      </c>
-      <c r="I40">
         <v>90</v>
       </c>
     </row>
@@ -1732,6 +1650,1100 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>12.5</v>
+      </c>
+      <c r="C2">
+        <v>23.5</v>
+      </c>
+      <c r="D2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E2">
+        <f>D2*1000</f>
+        <v>2300</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>0.1</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>23.3</v>
+      </c>
+      <c r="C3">
+        <v>8.9</v>
+      </c>
+      <c r="D3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E3">
+        <f>D3*1000</f>
+        <v>2200</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>0.1</v>
+      </c>
+      <c r="H3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>26.3</v>
+      </c>
+      <c r="C4">
+        <v>14.2</v>
+      </c>
+      <c r="D4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E4">
+        <f>D4*1000</f>
+        <v>2300</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>0.1</v>
+      </c>
+      <c r="H4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>11.5</v>
+      </c>
+      <c r="C5">
+        <v>23</v>
+      </c>
+      <c r="D5">
+        <v>2.1</v>
+      </c>
+      <c r="E5">
+        <f>D5*1000</f>
+        <v>2100</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>0.1</v>
+      </c>
+      <c r="H5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>29.6</v>
+      </c>
+      <c r="C6">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="D6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E6">
+        <f>D6*1000</f>
+        <v>2300</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>0.1</v>
+      </c>
+      <c r="H6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>23.2</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E7">
+        <f>D7*1000</f>
+        <v>2200</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>0.1</v>
+      </c>
+      <c r="H7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>26.8</v>
+      </c>
+      <c r="C8">
+        <v>6.4</v>
+      </c>
+      <c r="D8">
+        <v>1.7</v>
+      </c>
+      <c r="E8">
+        <f>D8*1000</f>
+        <v>1700</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>0.1</v>
+      </c>
+      <c r="H8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="C9">
+        <v>11.6</v>
+      </c>
+      <c r="D9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E9">
+        <f>D9*1000</f>
+        <v>2300</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>0.1</v>
+      </c>
+      <c r="H9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>91</v>
+      </c>
+      <c r="C10">
+        <v>4.8</v>
+      </c>
+      <c r="D10">
+        <v>1.5</v>
+      </c>
+      <c r="E10">
+        <f>D10*1000</f>
+        <v>1500</v>
+      </c>
+      <c r="F10">
+        <v>17</v>
+      </c>
+      <c r="G10">
+        <v>0.1</v>
+      </c>
+      <c r="H10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>92.8</v>
+      </c>
+      <c r="C11">
+        <v>5.5</v>
+      </c>
+      <c r="D11">
+        <v>1.7</v>
+      </c>
+      <c r="E11">
+        <f>D11*1000</f>
+        <v>1700</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11">
+        <v>0.1</v>
+      </c>
+      <c r="H11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12">
+        <v>93.1</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>1.5</v>
+      </c>
+      <c r="E12">
+        <f>D12*1000</f>
+        <v>1500</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>0.1</v>
+      </c>
+      <c r="H12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>92.9</v>
+      </c>
+      <c r="C13">
+        <v>6.2</v>
+      </c>
+      <c r="D13">
+        <v>1.5</v>
+      </c>
+      <c r="E13">
+        <f>D13*1000</f>
+        <v>1500</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>0.1</v>
+      </c>
+      <c r="H13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14">
+        <v>85.5</v>
+      </c>
+      <c r="C14">
+        <v>6.6</v>
+      </c>
+      <c r="D14">
+        <v>1.8</v>
+      </c>
+      <c r="E14">
+        <f>D14*1000</f>
+        <v>1800</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>0.1</v>
+      </c>
+      <c r="H14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15">
+        <v>91.5</v>
+      </c>
+      <c r="C15">
+        <v>3.7</v>
+      </c>
+      <c r="D15">
+        <v>1.9</v>
+      </c>
+      <c r="E15">
+        <f>D15*1000</f>
+        <v>1900</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>0.1</v>
+      </c>
+      <c r="H15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16">
+        <v>91.9</v>
+      </c>
+      <c r="C16">
+        <v>3.9</v>
+      </c>
+      <c r="D16">
+        <v>1.5</v>
+      </c>
+      <c r="E16">
+        <f>D16*1000</f>
+        <v>1500</v>
+      </c>
+      <c r="F16">
+        <v>15</v>
+      </c>
+      <c r="G16">
+        <v>0.1</v>
+      </c>
+      <c r="H16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>87.3</v>
+      </c>
+      <c r="C17">
+        <v>9.1</v>
+      </c>
+      <c r="D17">
+        <v>3.2</v>
+      </c>
+      <c r="E17">
+        <f>D17*1000</f>
+        <v>3200</v>
+      </c>
+      <c r="F17">
+        <v>75</v>
+      </c>
+      <c r="G17">
+        <v>0.1</v>
+      </c>
+      <c r="H17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>87</v>
+      </c>
+      <c r="C18">
+        <v>14.4</v>
+      </c>
+      <c r="D18">
+        <v>3.2</v>
+      </c>
+      <c r="E18">
+        <f>D18*1000</f>
+        <v>3200</v>
+      </c>
+      <c r="F18">
+        <v>100</v>
+      </c>
+      <c r="G18">
+        <v>0.1</v>
+      </c>
+      <c r="H18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>89.6</v>
+      </c>
+      <c r="C19">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D19">
+        <v>3.1</v>
+      </c>
+      <c r="E19">
+        <f>D19*1000</f>
+        <v>3100</v>
+      </c>
+      <c r="F19">
+        <v>100</v>
+      </c>
+      <c r="G19">
+        <v>0.1</v>
+      </c>
+      <c r="H19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20">
+        <v>87.5</v>
+      </c>
+      <c r="C20">
+        <v>12.8</v>
+      </c>
+      <c r="D20">
+        <v>2.9</v>
+      </c>
+      <c r="E20">
+        <f>D20*1000</f>
+        <v>2900</v>
+      </c>
+      <c r="F20">
+        <v>50</v>
+      </c>
+      <c r="G20">
+        <v>0.1</v>
+      </c>
+      <c r="H20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21">
+        <v>89</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>2.6</v>
+      </c>
+      <c r="E21">
+        <f>D21*1000</f>
+        <v>2600</v>
+      </c>
+      <c r="F21">
+        <v>50</v>
+      </c>
+      <c r="G21">
+        <v>0.1</v>
+      </c>
+      <c r="H21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>87</v>
+      </c>
+      <c r="C22">
+        <v>15.9</v>
+      </c>
+      <c r="D22">
+        <v>2.8</v>
+      </c>
+      <c r="E22">
+        <f>D22*1000</f>
+        <v>2800</v>
+      </c>
+      <c r="F22">
+        <v>45</v>
+      </c>
+      <c r="G22">
+        <v>0.1</v>
+      </c>
+      <c r="H22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23">
+        <v>90.2</v>
+      </c>
+      <c r="C23">
+        <v>15.9</v>
+      </c>
+      <c r="D23">
+        <v>2.8</v>
+      </c>
+      <c r="E23">
+        <f>D23*1000</f>
+        <v>2800</v>
+      </c>
+      <c r="F23">
+        <v>30</v>
+      </c>
+      <c r="G23">
+        <v>0.1</v>
+      </c>
+      <c r="H23">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>10.7</v>
+      </c>
+      <c r="D24">
+        <v>2.4</v>
+      </c>
+      <c r="E24">
+        <f>D24*1000</f>
+        <v>2400</v>
+      </c>
+      <c r="F24">
+        <v>50</v>
+      </c>
+      <c r="G24">
+        <v>0.1</v>
+      </c>
+      <c r="H24">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25">
+        <v>20.8</v>
+      </c>
+      <c r="C25">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D25">
+        <v>2.1</v>
+      </c>
+      <c r="E25">
+        <f>D25*1000</f>
+        <v>2100</v>
+      </c>
+      <c r="F25">
+        <v>20</v>
+      </c>
+      <c r="G25">
+        <v>0.1</v>
+      </c>
+      <c r="H25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26">
+        <v>23</v>
+      </c>
+      <c r="C26">
+        <v>10.3</v>
+      </c>
+      <c r="D26">
+        <v>2.5</v>
+      </c>
+      <c r="E26">
+        <f>D26*1000</f>
+        <v>2500</v>
+      </c>
+      <c r="F26">
+        <v>20</v>
+      </c>
+      <c r="G26">
+        <v>0.1</v>
+      </c>
+      <c r="H26">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27">
+        <v>89</v>
+      </c>
+      <c r="C27">
+        <v>15.3</v>
+      </c>
+      <c r="D27">
+        <v>2.4</v>
+      </c>
+      <c r="E27">
+        <f>D27*1000</f>
+        <v>2400</v>
+      </c>
+      <c r="F27">
+        <v>65</v>
+      </c>
+      <c r="G27">
+        <v>0.1</v>
+      </c>
+      <c r="H27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28">
+        <v>88.6</v>
+      </c>
+      <c r="C28">
+        <v>16.8</v>
+      </c>
+      <c r="D28">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E28">
+        <f>D28*1000</f>
+        <v>2300</v>
+      </c>
+      <c r="F28">
+        <v>65</v>
+      </c>
+      <c r="G28">
+        <v>0.1</v>
+      </c>
+      <c r="H28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29">
+        <v>87.9</v>
+      </c>
+      <c r="C29">
+        <v>17.5</v>
+      </c>
+      <c r="D29">
+        <v>2.5</v>
+      </c>
+      <c r="E29">
+        <f>D29*1000</f>
+        <v>2500</v>
+      </c>
+      <c r="F29">
+        <v>65</v>
+      </c>
+      <c r="G29">
+        <v>0.1</v>
+      </c>
+      <c r="H29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30">
+        <v>84</v>
+      </c>
+      <c r="C30">
+        <v>3.5</v>
+      </c>
+      <c r="D30">
+        <v>2.5</v>
+      </c>
+      <c r="E30">
+        <f>D30*1000</f>
+        <v>2500</v>
+      </c>
+      <c r="F30">
+        <v>20</v>
+      </c>
+      <c r="G30">
+        <v>0.1</v>
+      </c>
+      <c r="H30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31">
+        <v>20.6</v>
+      </c>
+      <c r="C31">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="D31">
+        <v>2.8</v>
+      </c>
+      <c r="E31">
+        <f>D31*1000</f>
+        <v>2800</v>
+      </c>
+      <c r="F31">
+        <v>20</v>
+      </c>
+      <c r="G31">
+        <v>0.1</v>
+      </c>
+      <c r="H31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32">
+        <v>92.2</v>
+      </c>
+      <c r="C32">
+        <v>23.8</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <f>D32*1000</f>
+        <v>2000</v>
+      </c>
+      <c r="F32">
+        <v>100</v>
+      </c>
+      <c r="G32">
+        <v>0.1</v>
+      </c>
+      <c r="H32">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33">
+        <v>87.9</v>
+      </c>
+      <c r="C33">
+        <v>48</v>
+      </c>
+      <c r="D33">
+        <v>2.1</v>
+      </c>
+      <c r="E33">
+        <f>D33*1000</f>
+        <v>2100</v>
+      </c>
+      <c r="F33">
+        <v>300</v>
+      </c>
+      <c r="G33">
+        <v>0.1</v>
+      </c>
+      <c r="H33">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34">
+        <v>88.8</v>
+      </c>
+      <c r="C34">
+        <v>39.6</v>
+      </c>
+      <c r="D34">
+        <v>2.5</v>
+      </c>
+      <c r="E34">
+        <f>D34*1000</f>
+        <v>2500</v>
+      </c>
+      <c r="F34">
+        <v>145</v>
+      </c>
+      <c r="G34">
+        <v>0.1</v>
+      </c>
+      <c r="H34">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35">
+        <v>89.9</v>
+      </c>
+      <c r="C35">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="D35">
+        <v>2.7</v>
+      </c>
+      <c r="E35">
+        <f>D35*1000</f>
+        <v>2700</v>
+      </c>
+      <c r="F35">
+        <v>130</v>
+      </c>
+      <c r="G35">
+        <v>0.1</v>
+      </c>
+      <c r="H35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>88.3</v>
+      </c>
+      <c r="C36">
+        <v>29</v>
+      </c>
+      <c r="D36">
+        <v>2.8</v>
+      </c>
+      <c r="E36">
+        <f>D36*1000</f>
+        <v>2800</v>
+      </c>
+      <c r="F36">
+        <v>61</v>
+      </c>
+      <c r="G36">
+        <v>0.1</v>
+      </c>
+      <c r="H36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37">
+        <v>90</v>
+      </c>
+      <c r="C37">
+        <v>59.7</v>
+      </c>
+      <c r="D37">
+        <v>2.8</v>
+      </c>
+      <c r="E37">
+        <f>D37*1000</f>
+        <v>2800</v>
+      </c>
+      <c r="F37">
+        <v>40</v>
+      </c>
+      <c r="G37">
+        <v>0.1</v>
+      </c>
+      <c r="H37">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38">
+        <v>91.2</v>
+      </c>
+      <c r="C38">
+        <v>17.8</v>
+      </c>
+      <c r="D38">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E38">
+        <f>D38*1000</f>
+        <v>2200</v>
+      </c>
+      <c r="F38">
+        <v>50</v>
+      </c>
+      <c r="G38">
+        <v>0.1</v>
+      </c>
+      <c r="H38">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39">
+        <v>89</v>
+      </c>
+      <c r="C39">
+        <v>32.5</v>
+      </c>
+      <c r="D39">
+        <v>2.1</v>
+      </c>
+      <c r="E39">
+        <f>D39*1000</f>
+        <v>2100</v>
+      </c>
+      <c r="F39">
+        <v>55</v>
+      </c>
+      <c r="G39">
+        <v>0.1</v>
+      </c>
+      <c r="H39">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40">
+        <v>95</v>
+      </c>
+      <c r="C40">
+        <v>40.4</v>
+      </c>
+      <c r="D40">
+        <v>2.7</v>
+      </c>
+      <c r="E40">
+        <f>D40*1000</f>
+        <v>2700</v>
+      </c>
+      <c r="F40">
+        <v>120</v>
+      </c>
+      <c r="G40">
+        <v>0.1</v>
+      </c>
+      <c r="H40">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G47"/>
   <sheetViews>

</xml_diff>